<commit_message>
Finished comparables analysis part
</commit_message>
<xml_diff>
--- a/resources/TAMID-Comparable-Analysis-Template.xlsx
+++ b/resources/TAMID-Comparable-Analysis-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lawrencelim/Projects/python-projects/pyfinny/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642803F1-9D59-C049-8F00-4891C9A68A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3F0BA0-B3C5-2440-AE8D-13F54C88FD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13520" yWindow="700" windowWidth="13520" windowHeight="8440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Public-Comps" sheetId="1" r:id="rId1"/>
@@ -787,6 +787,8 @@
     <xf numFmtId="165" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -797,8 +799,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1017,7 +1017,7 @@
   <dimension ref="A1:AK1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1202,12 +1202,12 @@
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="89" t="s">
+      <c r="E5" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="91"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="93"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -1257,32 +1257,32 @@
       <c r="H6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="89" t="s">
+      <c r="I6" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="90"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="89" t="s">
+      <c r="J6" s="92"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="90"/>
-      <c r="N6" s="91"/>
-      <c r="O6" s="89" t="s">
+      <c r="M6" s="92"/>
+      <c r="N6" s="93"/>
+      <c r="O6" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="90"/>
-      <c r="Q6" s="91"/>
+      <c r="P6" s="92"/>
+      <c r="Q6" s="93"/>
       <c r="R6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="S6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="T6" s="89" t="s">
+      <c r="T6" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="U6" s="90"/>
-      <c r="V6" s="91"/>
+      <c r="U6" s="92"/>
+      <c r="V6" s="93"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
@@ -1399,7 +1399,7 @@
       <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="95">
+      <c r="D8" s="89">
         <v>18.899999999999999</v>
       </c>
       <c r="E8" s="85">
@@ -1483,7 +1483,7 @@
       <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="96">
+      <c r="D9" s="90">
         <v>49.03</v>
       </c>
       <c r="E9" s="86">
@@ -1567,7 +1567,7 @@
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="96">
+      <c r="D10" s="90">
         <v>15.5</v>
       </c>
       <c r="E10" s="86">
@@ -1651,7 +1651,7 @@
       <c r="C11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="96">
+      <c r="D11" s="90">
         <v>4.3499999999999996</v>
       </c>
       <c r="E11" s="86">
@@ -1735,7 +1735,7 @@
       <c r="C12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="96">
+      <c r="D12" s="90">
         <v>43.29</v>
       </c>
       <c r="E12" s="86">
@@ -1819,7 +1819,7 @@
       <c r="C13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="96">
+      <c r="D13" s="90">
         <v>72.510000000000005</v>
       </c>
       <c r="E13" s="86">
@@ -2569,22 +2569,22 @@
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="89" t="s">
+      <c r="E23" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="90"/>
-      <c r="G23" s="90"/>
-      <c r="H23" s="91"/>
-      <c r="I23" s="89" t="s">
+      <c r="F23" s="92"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="93"/>
+      <c r="I23" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="J23" s="90"/>
-      <c r="K23" s="91"/>
-      <c r="L23" s="89" t="s">
+      <c r="J23" s="92"/>
+      <c r="K23" s="93"/>
+      <c r="L23" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="M23" s="90"/>
-      <c r="N23" s="91"/>
+      <c r="M23" s="92"/>
+      <c r="N23" s="93"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
@@ -2622,21 +2622,21 @@
       <c r="H24" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="89" t="s">
+      <c r="I24" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="90"/>
-      <c r="K24" s="91"/>
-      <c r="L24" s="89" t="s">
+      <c r="J24" s="92"/>
+      <c r="K24" s="93"/>
+      <c r="L24" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="M24" s="90"/>
-      <c r="N24" s="91"/>
-      <c r="O24" s="89" t="s">
+      <c r="M24" s="92"/>
+      <c r="N24" s="93"/>
+      <c r="O24" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="P24" s="90"/>
-      <c r="Q24" s="91"/>
+      <c r="P24" s="92"/>
+      <c r="Q24" s="93"/>
       <c r="R24" s="49"/>
       <c r="S24" s="49"/>
       <c r="T24" s="49"/>
@@ -41205,17 +41205,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="T6:V6"/>
     <mergeCell ref="O24:Q24"/>
     <mergeCell ref="E23:H23"/>
     <mergeCell ref="L23:N23"/>
     <mergeCell ref="I23:K23"/>
     <mergeCell ref="I24:K24"/>
     <mergeCell ref="L24:N24"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="T6:V6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup scale="37" orientation="portrait"/>
@@ -41361,21 +41361,21 @@
       <c r="B5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="C5" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="89" t="s">
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="91"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="93"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -42177,15 +42177,15 @@
         <v>0</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="92" t="s">
+      <c r="G22" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="H22" s="93"/>
-      <c r="I22" s="93"/>
-      <c r="J22" s="93"/>
-      <c r="K22" s="93"/>
-      <c r="L22" s="93"/>
-      <c r="M22" s="94"/>
+      <c r="H22" s="95"/>
+      <c r="I22" s="95"/>
+      <c r="J22" s="95"/>
+      <c r="K22" s="95"/>
+      <c r="L22" s="95"/>
+      <c r="M22" s="96"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>

</xml_diff>